<commit_message>
Added anova support for distance and loudness
corrected some loudness anova scritpts and added support for distance
</commit_message>
<xml_diff>
--- a/matlab/statistics/DthdRanalysis.xlsx
+++ b/matlab/statistics/DthdRanalysis.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0FD3BF-EDAA-4A0A-8641-CDBD4B6674A2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3595840-1019-4EFA-BB05-661890CCBDF6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -121,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -133,6 +133,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -467,7 +468,10 @@
       <c r="F2" s="1">
         <v>16.1074729458918</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="5">
+        <v>174.8998</v>
+      </c>
+      <c r="K2" s="2">
         <v>174.9</v>
       </c>
     </row>
@@ -490,7 +494,10 @@
       <c r="F3" s="1">
         <v>15.512796593186399</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="5">
+        <v>170.8417</v>
+      </c>
+      <c r="K3" s="2">
         <v>170.8</v>
       </c>
     </row>
@@ -513,7 +520,10 @@
       <c r="F4" s="1">
         <v>16.268989979959901</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="5">
+        <v>160.92179999999999</v>
+      </c>
+      <c r="K4" s="2">
         <v>160.9</v>
       </c>
     </row>
@@ -536,7 +546,10 @@
       <c r="F5" s="1">
         <v>15.879880761522999</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="5">
+        <v>173.09620000000001</v>
+      </c>
+      <c r="K5" s="2">
         <v>173.1</v>
       </c>
     </row>
@@ -559,7 +572,10 @@
       <c r="F6" s="1">
         <v>15.109004008016001</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="5">
+        <v>188.42689999999999</v>
+      </c>
+      <c r="K6" s="2">
         <v>188.4</v>
       </c>
       <c r="O6" s="4" t="s">
@@ -585,7 +601,10 @@
       <c r="F7" s="1">
         <v>16.7535410821643</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="5">
+        <v>169.03809999999999</v>
+      </c>
+      <c r="K7" s="2">
         <v>169</v>
       </c>
     </row>
@@ -608,7 +627,10 @@
       <c r="F8" s="1">
         <v>18.126435871743499</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="5">
+        <v>119.88979999999999</v>
+      </c>
+      <c r="K8" s="2">
         <v>119.9</v>
       </c>
     </row>
@@ -631,7 +653,10 @@
       <c r="F9" s="1">
         <v>16.408481963927901</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="5">
+        <v>172.64529999999999</v>
+      </c>
+      <c r="K9" s="2">
         <v>172.6</v>
       </c>
     </row>
@@ -654,7 +679,10 @@
       <c r="F10" s="1">
         <v>16.408481963927901</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="5">
+        <v>50</v>
+      </c>
+      <c r="K10" s="3">
         <v>172.6</v>
       </c>
     </row>
@@ -677,7 +705,10 @@
       <c r="F11" s="1">
         <v>15.872539078156301</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="5">
+        <v>171.74350000000001</v>
+      </c>
+      <c r="K11" s="2">
         <v>171.7</v>
       </c>
     </row>
@@ -700,7 +731,10 @@
       <c r="F12" s="1">
         <v>20.651974949899799</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="5">
+        <v>72.094200000000001</v>
+      </c>
+      <c r="K12" s="2">
         <v>72.099999999999994</v>
       </c>
     </row>
@@ -723,7 +757,10 @@
       <c r="F13" s="1">
         <v>15.7844388777555</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="5">
+        <v>159.1182</v>
+      </c>
+      <c r="K13" s="2">
         <v>159.1</v>
       </c>
     </row>
@@ -746,7 +783,10 @@
       <c r="F14" s="1">
         <v>17.274800601202401</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="5">
+        <v>145.59119999999999</v>
+      </c>
+      <c r="K14" s="2">
         <v>145.6</v>
       </c>
     </row>
@@ -769,7 +809,10 @@
       <c r="F15" s="1">
         <v>16.9884749498998</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="5">
+        <v>147.84569999999999</v>
+      </c>
+      <c r="K15" s="2">
         <v>147.80000000000001</v>
       </c>
     </row>
@@ -792,11 +835,14 @@
       <c r="F16" s="1">
         <v>16.966449899799599</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="5">
+        <v>144.68940000000001</v>
+      </c>
+      <c r="K16" s="2">
         <v>144.69999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -815,11 +861,14 @@
       <c r="F17" s="1">
         <v>18.309977955911801</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="5">
+        <v>130.7114</v>
+      </c>
+      <c r="K17" s="2">
         <v>130.69999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -838,11 +887,14 @@
       <c r="F18" s="1">
         <v>15.696338677354699</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="5">
+        <v>178.9579</v>
+      </c>
+      <c r="K18" s="2">
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -861,11 +913,14 @@
       <c r="F19" s="1">
         <v>17.942893787575201</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="5">
+        <v>136.57310000000001</v>
+      </c>
+      <c r="K19" s="2">
         <v>136.6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -884,11 +939,14 @@
       <c r="F20" s="1">
         <v>16.349748496994</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="5">
+        <v>181.66329999999999</v>
+      </c>
+      <c r="K20" s="2">
         <v>181.7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -907,11 +965,14 @@
       <c r="F21" s="1">
         <v>16.349748496994</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="5">
+        <v>50</v>
+      </c>
+      <c r="K21" s="3">
         <v>181.7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -930,11 +991,14 @@
       <c r="F22" s="1">
         <v>43.7989509018036</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="5">
+        <v>165.43090000000001</v>
+      </c>
+      <c r="K22" s="2">
         <v>165.4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -953,11 +1017,14 @@
       <c r="F23" s="1">
         <v>43.562648296593203</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="5">
+        <v>173.09620000000001</v>
+      </c>
+      <c r="K23" s="2">
         <v>173.1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -976,11 +1043,14 @@
       <c r="F24" s="1">
         <v>43.9879929859719</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="5">
+        <v>171.74350000000001</v>
+      </c>
+      <c r="K24" s="2">
         <v>171.7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -999,11 +1069,14 @@
       <c r="F25" s="1">
         <v>44.366077154308599</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="5">
+        <v>169.93989999999999</v>
+      </c>
+      <c r="K25" s="2">
         <v>169.9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1022,11 +1095,14 @@
       <c r="F26" s="1">
         <v>43.090043086172301</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="5">
+        <v>174.8998</v>
+      </c>
+      <c r="K26" s="2">
         <v>174.9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1045,11 +1121,14 @@
       <c r="F27" s="1">
         <v>43.775320641282597</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="5">
+        <v>175.80160000000001</v>
+      </c>
+      <c r="K27" s="2">
         <v>175.8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1068,11 +1147,14 @@
       <c r="F28" s="1">
         <v>43.775320641282597</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="5">
+        <v>224.499</v>
+      </c>
+      <c r="K28" s="2">
         <v>224.5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1091,11 +1173,14 @@
       <c r="F29" s="1">
         <v>46.232867735470997</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="5">
+        <v>147.84569999999999</v>
+      </c>
+      <c r="K29" s="2">
         <v>147.80000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1114,11 +1199,14 @@
       <c r="F30" s="1">
         <v>51.431525050100198</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="5">
+        <v>121.6934</v>
+      </c>
+      <c r="K30" s="2">
         <v>121.7</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1137,11 +1225,14 @@
       <c r="F31" s="1">
         <v>44.0588837675351</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="5">
+        <v>176.2525</v>
+      </c>
+      <c r="K31" s="2">
         <v>176.3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1160,11 +1251,14 @@
       <c r="F32" s="1">
         <v>43.255454909819598</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="5">
+        <v>193.83770000000001</v>
+      </c>
+      <c r="K32" s="2">
         <v>193.8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1183,11 +1277,14 @@
       <c r="F33" s="1">
         <v>42.735589178356697</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="5">
+        <v>198.3467</v>
+      </c>
+      <c r="K33" s="2">
         <v>198.3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1206,11 +1303,14 @@
       <c r="F34" s="1">
         <v>41.577706412825698</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="5">
+        <v>173.5471</v>
+      </c>
+      <c r="K34" s="2">
         <v>173.5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1229,11 +1329,14 @@
       <c r="F35" s="1">
         <v>43.775320641282597</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="5">
+        <v>196.09219999999999</v>
+      </c>
+      <c r="K35" s="2">
         <v>196.1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1252,11 +1355,14 @@
       <c r="F36" s="1">
         <v>43.208194388777599</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="5">
+        <v>178.05609999999999</v>
+      </c>
+      <c r="K36" s="2">
         <v>178.1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1275,11 +1381,14 @@
       <c r="F37" s="1">
         <v>43.0191523046092</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="5">
+        <v>194.2886</v>
+      </c>
+      <c r="K37" s="2">
         <v>194.3</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1298,11 +1407,14 @@
       <c r="F38" s="1">
         <v>45.098615230460901</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="5">
+        <v>160.4709</v>
+      </c>
+      <c r="K38" s="2">
         <v>160.5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1321,11 +1433,14 @@
       <c r="F39" s="1">
         <v>49.682885771543098</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="5">
+        <v>134.76949999999999</v>
+      </c>
+      <c r="K39" s="2">
         <v>134.80000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1344,11 +1459,14 @@
       <c r="F40" s="1">
         <v>49.682885771543098</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="5">
+        <v>202.40479999999999</v>
+      </c>
+      <c r="K40" s="2">
         <v>202.4</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1367,11 +1485,14 @@
       <c r="F41" s="1">
         <v>49.682885771543098</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="5">
+        <v>50</v>
+      </c>
+      <c r="K41" s="3">
         <v>202.4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1390,11 +1511,14 @@
       <c r="F42" s="1">
         <v>52.313152304609197</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="5">
+        <v>172.1944</v>
+      </c>
+      <c r="K42" s="2">
         <v>172.2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1413,11 +1537,14 @@
       <c r="F43" s="1">
         <v>50.460655310621199</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="5">
+        <v>202.40479999999999</v>
+      </c>
+      <c r="K43" s="2">
         <v>202.4</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1436,11 +1563,14 @@
       <c r="F44" s="1">
         <v>54.979625250501002</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="5">
+        <v>198.3467</v>
+      </c>
+      <c r="K44" s="2">
         <v>198.3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1459,11 +1589,14 @@
       <c r="F45" s="1">
         <v>51.134290581162297</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="5">
+        <v>182.5651</v>
+      </c>
+      <c r="K45" s="2">
         <v>182.6</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1482,11 +1615,14 @@
       <c r="F46" s="1">
         <v>50.544859719438897</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="5">
+        <v>188.87780000000001</v>
+      </c>
+      <c r="K46" s="2">
         <v>188.9</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1505,11 +1641,14 @@
       <c r="F47" s="1">
         <v>49.955428857715397</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="5">
+        <v>209.61920000000001</v>
+      </c>
+      <c r="K47" s="2">
         <v>209.6</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1528,11 +1667,14 @@
       <c r="F48" s="1">
         <v>48.692362725450899</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="5">
+        <v>196.09219999999999</v>
+      </c>
+      <c r="K48" s="2">
         <v>196.1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1551,11 +1693,14 @@
       <c r="F49" s="1">
         <v>58.656551102204403</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49" s="5">
+        <v>146.0421</v>
+      </c>
+      <c r="K49" s="2">
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1574,11 +1719,14 @@
       <c r="F50" s="1">
         <v>52.116675350701399</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G50" s="5">
+        <v>192.0341</v>
+      </c>
+      <c r="K50" s="2">
         <v>192</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1597,11 +1745,14 @@
       <c r="F51" s="1">
         <v>52.4815611222445</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G51" s="5">
+        <v>169.93989999999999</v>
+      </c>
+      <c r="K51" s="2">
         <v>169.9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -1620,11 +1771,14 @@
       <c r="F52" s="1">
         <v>53.014855711422904</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G52" s="5">
+        <v>167.68539999999999</v>
+      </c>
+      <c r="K52" s="2">
         <v>167.7</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -1643,11 +1797,14 @@
       <c r="F53" s="1">
         <v>52.341220440881798</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G53" s="5">
+        <v>166.78360000000001</v>
+      </c>
+      <c r="K53" s="2">
         <v>166.8</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -1666,11 +1823,14 @@
       <c r="F54" s="1">
         <v>51.864062124248498</v>
       </c>
-      <c r="G54" s="2">
+      <c r="G54" s="5">
+        <v>169.03809999999999</v>
+      </c>
+      <c r="K54" s="2">
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -1689,11 +1849,14 @@
       <c r="F55" s="1">
         <v>50.769404809619203</v>
       </c>
-      <c r="G55" s="2">
+      <c r="G55" s="5">
+        <v>208.7174</v>
+      </c>
+      <c r="K55" s="2">
         <v>208.7</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -1712,11 +1875,14 @@
       <c r="F56" s="1">
         <v>53.688490981963902</v>
       </c>
-      <c r="G56" s="2">
+      <c r="G56" s="5">
+        <v>151.4529</v>
+      </c>
+      <c r="K56" s="2">
         <v>151.5</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -1735,11 +1901,14 @@
       <c r="F57" s="1">
         <v>53.014855711422797</v>
       </c>
-      <c r="G57" s="2">
+      <c r="G57" s="5">
+        <v>200.15029999999999</v>
+      </c>
+      <c r="K57" s="2">
         <v>200.2</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -1758,11 +1927,14 @@
       <c r="F58" s="1">
         <v>53.7726953907816</v>
       </c>
-      <c r="G58" s="2">
+      <c r="G58" s="5">
+        <v>169.489</v>
+      </c>
+      <c r="K58" s="2">
         <v>169.5</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -1781,11 +1953,14 @@
       <c r="F59" s="1">
         <v>51.639517034068099</v>
       </c>
-      <c r="G59" s="2">
+      <c r="G59" s="5">
+        <v>198.79759999999999</v>
+      </c>
+      <c r="K59" s="2">
         <v>198.8</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -1804,11 +1979,14 @@
       <c r="F60" s="1">
         <v>48.748498997996002</v>
       </c>
-      <c r="G60" s="2">
+      <c r="G60" s="5">
+        <v>210.0701</v>
+      </c>
+      <c r="K60" s="2">
         <v>210.1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -1827,11 +2005,14 @@
       <c r="F61" s="1">
         <v>57.758370741482999</v>
       </c>
-      <c r="G61" s="2">
+      <c r="G61" s="5">
+        <v>146.0421</v>
+      </c>
+      <c r="K61" s="2">
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -1850,11 +2031,14 @@
       <c r="F62" s="1">
         <v>22.592955911823601</v>
       </c>
-      <c r="G62" s="2">
+      <c r="G62" s="5">
+        <v>168.5872</v>
+      </c>
+      <c r="K62" s="2">
         <v>168.6</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -1873,11 +2057,14 @@
       <c r="F63" s="1">
         <v>22.686456913827701</v>
       </c>
-      <c r="G63" s="2">
+      <c r="G63" s="5">
+        <v>167.2345</v>
+      </c>
+      <c r="K63" s="2">
         <v>167.2</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -1896,11 +2083,14 @@
       <c r="F64" s="1">
         <v>22.571378757514999</v>
       </c>
-      <c r="G64" s="2">
+      <c r="G64" s="5">
+        <v>173.99799999999999</v>
+      </c>
+      <c r="K64" s="2">
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -1919,11 +2109,14 @@
       <c r="F65" s="1">
         <v>22.2692985971944</v>
       </c>
-      <c r="G65" s="2">
+      <c r="G65" s="5">
+        <v>207.3647</v>
+      </c>
+      <c r="K65" s="2">
         <v>207.4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -1942,11 +2135,14 @@
       <c r="F66" s="1">
         <v>22.2692985971944</v>
       </c>
-      <c r="G66" s="2">
+      <c r="G66" s="5">
+        <v>163.1764</v>
+      </c>
+      <c r="K66" s="2">
         <v>163.19999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -1965,11 +2161,14 @@
       <c r="F67" s="1">
         <v>22.197374749499001</v>
       </c>
-      <c r="G67" s="2">
+      <c r="G67" s="5">
+        <v>213.22649999999999</v>
+      </c>
+      <c r="K67" s="2">
         <v>213.2</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -1988,11 +2187,14 @@
       <c r="F68" s="1">
         <v>21.693907815631299</v>
       </c>
-      <c r="G68" s="2">
+      <c r="G68" s="5">
+        <v>216.3828</v>
+      </c>
+      <c r="K68" s="2">
         <v>216.4</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2011,11 +2213,14 @@
       <c r="F69" s="1">
         <v>22.060719438877801</v>
       </c>
-      <c r="G69" s="2">
+      <c r="G69" s="5">
+        <v>173.99799999999999</v>
+      </c>
+      <c r="K69" s="2">
         <v>174</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2034,11 +2239,14 @@
       <c r="F70" s="1">
         <v>25.628142284569101</v>
       </c>
-      <c r="G70" s="3">
+      <c r="G70" s="5">
+        <v>50</v>
+      </c>
+      <c r="K70" s="3">
         <v>174</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2057,11 +2265,14 @@
       <c r="F71" s="1">
         <v>22.571378757514999</v>
       </c>
-      <c r="G71" s="2">
+      <c r="G71" s="5">
+        <v>184.81960000000001</v>
+      </c>
+      <c r="K71" s="2">
         <v>184.8</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2080,11 +2291,14 @@
       <c r="F72" s="1">
         <v>22.7511883767535</v>
       </c>
-      <c r="G72" s="2">
+      <c r="G72" s="5">
+        <v>153.25649999999999</v>
+      </c>
+      <c r="K72" s="2">
         <v>153.30000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2103,11 +2317,14 @@
       <c r="F73" s="1">
         <v>22.190182364729498</v>
       </c>
-      <c r="G73" s="2">
+      <c r="G73" s="5">
+        <v>187.976</v>
+      </c>
+      <c r="K73" s="2">
         <v>188</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -2126,11 +2343,14 @@
       <c r="F74" s="1">
         <v>22.190182364729498</v>
       </c>
-      <c r="G74" s="2">
+      <c r="G74" s="5">
+        <v>182.5651</v>
+      </c>
+      <c r="K74" s="2">
         <v>182.6</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -2149,11 +2369,14 @@
       <c r="F75" s="1">
         <v>23.305002004007999</v>
       </c>
-      <c r="G75" s="2">
+      <c r="G75" s="5">
+        <v>144.23849999999999</v>
+      </c>
+      <c r="K75" s="2">
         <v>144.19999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -2172,11 +2395,14 @@
       <c r="F76" s="1">
         <v>21.600406813627298</v>
       </c>
-      <c r="G76" s="2">
+      <c r="G76" s="5">
+        <v>211.87370000000001</v>
+      </c>
+      <c r="K76" s="2">
         <v>211.9</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -2195,11 +2421,14 @@
       <c r="F77" s="1">
         <v>21.600406813627298</v>
       </c>
-      <c r="G77" s="3">
+      <c r="G77" s="5">
+        <v>50</v>
+      </c>
+      <c r="K77" s="3">
         <v>211.9</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -2218,11 +2447,14 @@
       <c r="F78" s="1">
         <v>21.600406813627298</v>
       </c>
-      <c r="G78" s="3">
+      <c r="G78" s="5">
+        <v>50</v>
+      </c>
+      <c r="K78" s="3">
         <v>211.9</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -2241,11 +2473,14 @@
       <c r="F79" s="1">
         <v>25.333254509018001</v>
       </c>
-      <c r="G79" s="2">
+      <c r="G79" s="5">
+        <v>88.326700000000002</v>
+      </c>
+      <c r="K79" s="2">
         <v>88.3</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -2264,11 +2499,14 @@
       <c r="F80" s="1">
         <v>22.672072144288599</v>
       </c>
-      <c r="G80" s="2">
+      <c r="G80" s="5">
+        <v>160.92179999999999</v>
+      </c>
+      <c r="K80" s="2">
         <v>160.9</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -2287,11 +2525,14 @@
       <c r="F81" s="1">
         <v>21.600406813627298</v>
       </c>
-      <c r="G81" s="3">
+      <c r="G81" s="5">
+        <v>50</v>
+      </c>
+      <c r="K81" s="3">
         <v>160.9</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -2310,11 +2551,14 @@
       <c r="F82" s="1">
         <v>49.742509018036102</v>
       </c>
-      <c r="G82" s="2">
+      <c r="G82" s="5">
+        <v>209.16829999999999</v>
+      </c>
+      <c r="K82" s="2">
         <v>209.2</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -2333,11 +2577,14 @@
       <c r="F83" s="1">
         <v>49.422511022044098</v>
       </c>
-      <c r="G83" s="2">
+      <c r="G83" s="5">
+        <v>178.9579</v>
+      </c>
+      <c r="K83" s="2">
         <v>179</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -2356,11 +2603,14 @@
       <c r="F84" s="1">
         <v>50.087122244489002</v>
       </c>
-      <c r="G84" s="2">
+      <c r="G84" s="5">
+        <v>184.36869999999999</v>
+      </c>
+      <c r="K84" s="2">
         <v>184.4</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -2379,11 +2629,14 @@
       <c r="F85" s="1">
         <v>45.927148296593202</v>
       </c>
-      <c r="G85" s="2">
+      <c r="G85" s="5">
+        <v>265.53109999999998</v>
+      </c>
+      <c r="K85" s="2">
         <v>265.5</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -2402,11 +2655,14 @@
       <c r="F86" s="1">
         <v>49.988661322645299</v>
       </c>
-      <c r="G86" s="2">
+      <c r="G86" s="5">
+        <v>175.35069999999999</v>
+      </c>
+      <c r="K86" s="2">
         <v>175.4</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -2425,11 +2681,14 @@
       <c r="F87" s="1">
         <v>47.724060120240502</v>
       </c>
-      <c r="G87" s="2">
+      <c r="G87" s="5">
+        <v>224.04810000000001</v>
+      </c>
+      <c r="K87" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -2448,11 +2707,14 @@
       <c r="F88" s="1">
         <v>46.6656052104208</v>
       </c>
-      <c r="G88" s="2">
+      <c r="G88" s="5">
+        <v>238.92789999999999</v>
+      </c>
+      <c r="K88" s="2">
         <v>238.9</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -2471,11 +2733,14 @@
       <c r="F89" s="1">
         <v>49.939430861723402</v>
       </c>
-      <c r="G89" s="2">
+      <c r="G89" s="5">
+        <v>170.39080000000001</v>
+      </c>
+      <c r="K89" s="2">
         <v>170.4</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -2494,11 +2759,14 @@
       <c r="F90" s="1">
         <v>59.6378316633267</v>
       </c>
-      <c r="G90" s="2">
+      <c r="G90" s="5">
+        <v>91.933899999999994</v>
+      </c>
+      <c r="K90" s="2">
         <v>91.9</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -2517,11 +2785,14 @@
       <c r="F91" s="1">
         <v>48.585593186372698</v>
       </c>
-      <c r="G91" s="2">
+      <c r="G91" s="5">
+        <v>192.0341</v>
+      </c>
+      <c r="K91" s="2">
         <v>192</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -2540,11 +2811,14 @@
       <c r="F92" s="1">
         <v>53.951713426853701</v>
       </c>
-      <c r="G92" s="2">
+      <c r="G92" s="5">
+        <v>138.82769999999999</v>
+      </c>
+      <c r="K92" s="2">
         <v>138.80000000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -2563,11 +2837,14 @@
       <c r="F93" s="1">
         <v>48.142519038076202</v>
       </c>
-      <c r="G93" s="2">
+      <c r="G93" s="5">
+        <v>216.83369999999999</v>
+      </c>
+      <c r="K93" s="2">
         <v>216.8</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -2586,11 +2863,14 @@
       <c r="F94" s="1">
         <v>50.357889779559102</v>
       </c>
-      <c r="G94" s="2">
+      <c r="G94" s="5">
+        <v>205.11019999999999</v>
+      </c>
+      <c r="K94" s="2">
         <v>205.1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -2609,11 +2889,14 @@
       <c r="F95" s="1">
         <v>52.647106212424802</v>
       </c>
-      <c r="G95" s="2">
+      <c r="G95" s="5">
+        <v>153.70740000000001</v>
+      </c>
+      <c r="K95" s="2">
         <v>153.69999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -2632,11 +2915,14 @@
       <c r="F96" s="1">
         <v>46.887142284569101</v>
       </c>
-      <c r="G96" s="2">
+      <c r="G96" s="5">
+        <v>233.96789999999999</v>
+      </c>
+      <c r="K96" s="2">
         <v>234</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -2655,11 +2941,14 @@
       <c r="F97" s="1">
         <v>56.216314629258498</v>
       </c>
-      <c r="G97" s="2">
+      <c r="G97" s="5">
+        <v>99.148300000000006</v>
+      </c>
+      <c r="K97" s="2">
         <v>99.1</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -2678,11 +2967,14 @@
       <c r="F98" s="1">
         <v>53.065565130260502</v>
       </c>
-      <c r="G98" s="2">
+      <c r="G98" s="5">
+        <v>170.8417</v>
+      </c>
+      <c r="K98" s="2">
         <v>170.8</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -2701,11 +2993,14 @@
       <c r="F99" s="1">
         <v>54.690170340681398</v>
       </c>
-      <c r="G99" s="2">
+      <c r="G99" s="5">
+        <v>127.5551</v>
+      </c>
+      <c r="K99" s="2">
         <v>127.6</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -2724,11 +3019,14 @@
       <c r="F100" s="1">
         <v>51.342498997996003</v>
       </c>
-      <c r="G100" s="2">
+      <c r="G100" s="5">
+        <v>165.43090000000001</v>
+      </c>
+      <c r="K100" s="2">
         <v>165.4</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -2747,11 +3045,14 @@
       <c r="F101" s="1">
         <v>51.342498997996003</v>
       </c>
-      <c r="G101" s="3">
+      <c r="G101" s="5">
+        <v>50</v>
+      </c>
+      <c r="K101" s="3">
         <v>165.4</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -2770,11 +3071,14 @@
       <c r="F102" s="1">
         <v>54.650919839679403</v>
       </c>
-      <c r="G102" s="2">
+      <c r="G102" s="5">
+        <v>224.04810000000001</v>
+      </c>
+      <c r="K102" s="2">
         <v>224</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -2793,11 +3097,14 @@
       <c r="F103" s="1">
         <v>53.0714408817635</v>
       </c>
-      <c r="G103" s="2">
+      <c r="G103" s="5">
+        <v>266.88380000000001</v>
+      </c>
+      <c r="K103" s="2">
         <v>266.89999999999998</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -2816,11 +3123,14 @@
       <c r="F104" s="1">
         <v>53.255713426853703</v>
       </c>
-      <c r="G104" s="2">
+      <c r="G104" s="5">
+        <v>270.0401</v>
+      </c>
+      <c r="K104" s="2">
         <v>270</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -2839,11 +3149,14 @@
       <c r="F105" s="1">
         <v>53.492635270541101</v>
       </c>
-      <c r="G105" s="2">
+      <c r="G105" s="5">
+        <v>256.96390000000002</v>
+      </c>
+      <c r="K105" s="2">
         <v>257</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -2862,11 +3175,14 @@
       <c r="F106" s="1">
         <v>53.282038076152297</v>
       </c>
-      <c r="G106" s="2">
+      <c r="G106" s="5">
+        <v>294.83969999999999</v>
+      </c>
+      <c r="K106" s="2">
         <v>294.8</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -2885,11 +3201,14 @@
       <c r="F107" s="1">
         <v>52.702895791583202</v>
       </c>
-      <c r="G107" s="2">
+      <c r="G107" s="5">
+        <v>304.30860000000001</v>
+      </c>
+      <c r="K107" s="2">
         <v>304.3</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -2908,11 +3227,14 @@
       <c r="F108" s="1">
         <v>53.361012024048101</v>
       </c>
-      <c r="G108" s="2">
+      <c r="G108" s="5">
+        <v>259.66930000000002</v>
+      </c>
+      <c r="K108" s="2">
         <v>259.7</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -2931,11 +3253,14 @@
       <c r="F109" s="1">
         <v>53.0714408817635</v>
       </c>
-      <c r="G109" s="2">
+      <c r="G109" s="5">
+        <v>274.09820000000002</v>
+      </c>
+      <c r="K109" s="2">
         <v>274.10000000000002</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -2954,11 +3279,14 @@
       <c r="F110" s="1">
         <v>53.097765531062102</v>
       </c>
-      <c r="G110" s="2">
+      <c r="G110" s="5">
         <v>275</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K110" s="2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -2977,11 +3305,14 @@
       <c r="F111" s="1">
         <v>57.388683366733503</v>
       </c>
-      <c r="G111" s="2">
+      <c r="G111" s="5">
+        <v>178.50700000000001</v>
+      </c>
+      <c r="K111" s="2">
         <v>178.5</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -3000,11 +3331,14 @@
       <c r="F112" s="1">
         <v>55.151088176352701</v>
       </c>
-      <c r="G112" s="2">
+      <c r="G112" s="5">
+        <v>218.63730000000001</v>
+      </c>
+      <c r="K112" s="2">
         <v>218.6</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -3023,11 +3357,14 @@
       <c r="F113" s="1">
         <v>56.177749498997997</v>
       </c>
-      <c r="G113" s="2">
+      <c r="G113" s="5">
+        <v>182.5651</v>
+      </c>
+      <c r="K113" s="2">
         <v>182.6</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -3046,11 +3383,14 @@
       <c r="F114" s="1">
         <v>53.992803607214398</v>
       </c>
-      <c r="G114" s="2">
+      <c r="G114" s="5">
+        <v>234.86969999999999</v>
+      </c>
+      <c r="K114" s="2">
         <v>234.9</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -3069,11 +3409,14 @@
       <c r="F115" s="1">
         <v>53.782206412825701</v>
       </c>
-      <c r="G115" s="2">
+      <c r="G115" s="5">
+        <v>257.41480000000001</v>
+      </c>
+      <c r="K115" s="2">
         <v>257.39999999999998</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -3092,11 +3435,14 @@
       <c r="F116" s="1">
         <v>53.729557114228498</v>
       </c>
-      <c r="G116" s="2">
+      <c r="G116" s="5">
+        <v>249.74950000000001</v>
+      </c>
+      <c r="K116" s="2">
         <v>249.7</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -3115,11 +3461,14 @@
       <c r="F117" s="1">
         <v>53.571609218436897</v>
       </c>
-      <c r="G117" s="2">
+      <c r="G117" s="5">
+        <v>250.2004</v>
+      </c>
+      <c r="K117" s="2">
         <v>250.2</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -3138,11 +3487,14 @@
       <c r="F118" s="1">
         <v>57.151761523046098</v>
       </c>
-      <c r="G118" s="2">
+      <c r="G118" s="5">
+        <v>192.0341</v>
+      </c>
+      <c r="K118" s="2">
         <v>192</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -3161,11 +3513,14 @@
       <c r="F119" s="1">
         <v>56.046126252504997</v>
       </c>
-      <c r="G119" s="2">
+      <c r="G119" s="5">
+        <v>186.6232</v>
+      </c>
+      <c r="K119" s="2">
         <v>186.6</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -3184,11 +3539,14 @@
       <c r="F120" s="1">
         <v>54.8615170340681</v>
       </c>
-      <c r="G120" s="2">
+      <c r="G120" s="5">
+        <v>218.63730000000001</v>
+      </c>
+      <c r="K120" s="2">
         <v>218.6</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -3207,7 +3565,10 @@
       <c r="F121" s="1">
         <v>71.483410110543701</v>
       </c>
-      <c r="G121" s="2">
+      <c r="G121" s="5">
+        <v>121.24250000000001</v>
+      </c>
+      <c r="K121" s="2">
         <v>121.2</v>
       </c>
     </row>

</xml_diff>